<commit_message>
added more requirements and removed extra content in spreadsheet
</commit_message>
<xml_diff>
--- a/Spreadsheets/Output_Sheet_Blank.xlsx
+++ b/Spreadsheets/Output_Sheet_Blank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackkelly/micronPro/micronPro-worker/Spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED74A62-8744-9A4E-B427-F1B95A2F4144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25F6DAD-A5D2-F841-94C3-4F6E0B3AB9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="24500" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4160" yWindow="2360" windowWidth="29020" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Date:</t>
   </si>
@@ -42,18 +42,12 @@
     <t>Scale</t>
   </si>
   <si>
-    <t>2.59</t>
-  </si>
-  <si>
     <t>Image Name</t>
   </si>
   <si>
     <t># Of Images</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>Threshold Method</t>
   </si>
   <si>
@@ -96,10 +90,22 @@
     <t>Software Version</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>Manual Inspections</t>
+  </si>
+  <si>
+    <t>3.0.1</t>
+  </si>
+  <si>
+    <t>Pores Oversized</t>
+  </si>
+  <si>
+    <t>Pores Inspected</t>
+  </si>
+  <si>
+    <t>% of pores within spec</t>
   </si>
 </sst>
 </file>
@@ -253,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -271,6 +277,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -286,23 +304,14 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,8 +632,8 @@
   </sheetPr>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,30 +651,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="47" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="17"/>
+      <c r="A2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
       <c r="L2"/>
       <c r="N2"/>
       <c r="O2"/>
@@ -674,43 +683,41 @@
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
     <row r="5" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="12">
-        <v>80</v>
-      </c>
-      <c r="F6" s="13"/>
+        <v>13</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
       <c r="I6"/>
       <c r="J6"/>
       <c r="L6"/>
@@ -721,51 +728,63 @@
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="B7" s="5"/>
       <c r="C7" s="1"/>
       <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.12</v>
-      </c>
-      <c r="F7" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5">
-        <v>2.59</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="1"/>
+      <c r="D9" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
     </row>
     <row r="10" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5">
-        <v>160</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="D12" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:15" ht="26" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
@@ -776,21 +795,21 @@
     </row>
     <row r="14" spans="1:15" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="9:15" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -929,15 +948,19 @@
       <c r="O55" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A13:G13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" orientation="portrait" r:id="rId1"/>

</xml_diff>